<commit_message>
graphs and statistics done
</commit_message>
<xml_diff>
--- a/data/ae.xlsx
+++ b/data/ae.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mykad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mykad\Desktop\space_environment_lab04\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341E0225-68D3-4888-9A43-4521527EB3BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258B48D2-B07A-476B-A9C8-872D88C14E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="1447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="1388">
   <si>
     <t>DATE</t>
   </si>
@@ -4186,183 +4186,6 @@
   </si>
   <si>
     <t>23:00:00.000</t>
-  </si>
-  <si>
-    <t>23:01:00.000</t>
-  </si>
-  <si>
-    <t>23:02:00.000</t>
-  </si>
-  <si>
-    <t>23:03:00.000</t>
-  </si>
-  <si>
-    <t>23:04:00.000</t>
-  </si>
-  <si>
-    <t>23:05:00.000</t>
-  </si>
-  <si>
-    <t>23:06:00.000</t>
-  </si>
-  <si>
-    <t>23:07:00.000</t>
-  </si>
-  <si>
-    <t>23:08:00.000</t>
-  </si>
-  <si>
-    <t>23:09:00.000</t>
-  </si>
-  <si>
-    <t>23:10:00.000</t>
-  </si>
-  <si>
-    <t>23:11:00.000</t>
-  </si>
-  <si>
-    <t>23:12:00.000</t>
-  </si>
-  <si>
-    <t>23:13:00.000</t>
-  </si>
-  <si>
-    <t>23:14:00.000</t>
-  </si>
-  <si>
-    <t>23:15:00.000</t>
-  </si>
-  <si>
-    <t>23:16:00.000</t>
-  </si>
-  <si>
-    <t>23:17:00.000</t>
-  </si>
-  <si>
-    <t>23:18:00.000</t>
-  </si>
-  <si>
-    <t>23:19:00.000</t>
-  </si>
-  <si>
-    <t>23:20:00.000</t>
-  </si>
-  <si>
-    <t>23:21:00.000</t>
-  </si>
-  <si>
-    <t>23:22:00.000</t>
-  </si>
-  <si>
-    <t>23:23:00.000</t>
-  </si>
-  <si>
-    <t>23:24:00.000</t>
-  </si>
-  <si>
-    <t>23:25:00.000</t>
-  </si>
-  <si>
-    <t>23:26:00.000</t>
-  </si>
-  <si>
-    <t>23:27:00.000</t>
-  </si>
-  <si>
-    <t>23:28:00.000</t>
-  </si>
-  <si>
-    <t>23:29:00.000</t>
-  </si>
-  <si>
-    <t>23:30:00.000</t>
-  </si>
-  <si>
-    <t>23:31:00.000</t>
-  </si>
-  <si>
-    <t>23:32:00.000</t>
-  </si>
-  <si>
-    <t>23:33:00.000</t>
-  </si>
-  <si>
-    <t>23:34:00.000</t>
-  </si>
-  <si>
-    <t>23:35:00.000</t>
-  </si>
-  <si>
-    <t>23:36:00.000</t>
-  </si>
-  <si>
-    <t>23:37:00.000</t>
-  </si>
-  <si>
-    <t>23:38:00.000</t>
-  </si>
-  <si>
-    <t>23:39:00.000</t>
-  </si>
-  <si>
-    <t>23:40:00.000</t>
-  </si>
-  <si>
-    <t>23:41:00.000</t>
-  </si>
-  <si>
-    <t>23:42:00.000</t>
-  </si>
-  <si>
-    <t>23:43:00.000</t>
-  </si>
-  <si>
-    <t>23:44:00.000</t>
-  </si>
-  <si>
-    <t>23:45:00.000</t>
-  </si>
-  <si>
-    <t>23:46:00.000</t>
-  </si>
-  <si>
-    <t>23:47:00.000</t>
-  </si>
-  <si>
-    <t>23:48:00.000</t>
-  </si>
-  <si>
-    <t>23:49:00.000</t>
-  </si>
-  <si>
-    <t>23:50:00.000</t>
-  </si>
-  <si>
-    <t>23:51:00.000</t>
-  </si>
-  <si>
-    <t>23:52:00.000</t>
-  </si>
-  <si>
-    <t>23:53:00.000</t>
-  </si>
-  <si>
-    <t>23:54:00.000</t>
-  </si>
-  <si>
-    <t>23:55:00.000</t>
-  </si>
-  <si>
-    <t>23:56:00.000</t>
-  </si>
-  <si>
-    <t>23:57:00.000</t>
-  </si>
-  <si>
-    <t>23:58:00.000</t>
-  </si>
-  <si>
-    <t>23:59:00.000</t>
   </si>
   <si>
     <t xml:space="preserve">AO     </t>
@@ -4696,10 +4519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1441"/>
+  <dimension ref="A1:G1382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A1371" workbookViewId="0">
+      <selection activeCell="K1380" sqref="K1380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4727,7 +4550,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>1446</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.3">
@@ -36491,1363 +36314,6 @@
       </c>
       <c r="G1382">
         <v>-75</v>
-      </c>
-    </row>
-    <row r="1383" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1383" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1383" t="s">
-        <v>1387</v>
-      </c>
-      <c r="C1383">
-        <v>7</v>
-      </c>
-      <c r="D1383">
-        <v>393</v>
-      </c>
-      <c r="E1383">
-        <v>109</v>
-      </c>
-      <c r="F1383">
-        <v>-284</v>
-      </c>
-      <c r="G1383">
-        <v>-88</v>
-      </c>
-    </row>
-    <row r="1384" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1384" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1384" t="s">
-        <v>1388</v>
-      </c>
-      <c r="C1384">
-        <v>7</v>
-      </c>
-      <c r="D1384">
-        <v>399</v>
-      </c>
-      <c r="E1384">
-        <v>121</v>
-      </c>
-      <c r="F1384">
-        <v>-278</v>
-      </c>
-      <c r="G1384">
-        <v>-79</v>
-      </c>
-    </row>
-    <row r="1385" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1385" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1385" t="s">
-        <v>1389</v>
-      </c>
-      <c r="C1385">
-        <v>7</v>
-      </c>
-      <c r="D1385">
-        <v>411</v>
-      </c>
-      <c r="E1385">
-        <v>121</v>
-      </c>
-      <c r="F1385">
-        <v>-290</v>
-      </c>
-      <c r="G1385">
-        <v>-85</v>
-      </c>
-    </row>
-    <row r="1386" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1386" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1386" t="s">
-        <v>1390</v>
-      </c>
-      <c r="C1386">
-        <v>7</v>
-      </c>
-      <c r="D1386">
-        <v>406</v>
-      </c>
-      <c r="E1386">
-        <v>111</v>
-      </c>
-      <c r="F1386">
-        <v>-295</v>
-      </c>
-      <c r="G1386">
-        <v>-92</v>
-      </c>
-    </row>
-    <row r="1387" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1387" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1387" t="s">
-        <v>1391</v>
-      </c>
-      <c r="C1387">
-        <v>7</v>
-      </c>
-      <c r="D1387">
-        <v>442</v>
-      </c>
-      <c r="E1387">
-        <v>107</v>
-      </c>
-      <c r="F1387">
-        <v>-335</v>
-      </c>
-      <c r="G1387">
-        <v>-114</v>
-      </c>
-    </row>
-    <row r="1388" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1388" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1388" t="s">
-        <v>1392</v>
-      </c>
-      <c r="C1388">
-        <v>7</v>
-      </c>
-      <c r="D1388">
-        <v>423</v>
-      </c>
-      <c r="E1388">
-        <v>111</v>
-      </c>
-      <c r="F1388">
-        <v>-312</v>
-      </c>
-      <c r="G1388">
-        <v>-101</v>
-      </c>
-    </row>
-    <row r="1389" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1389" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1389" t="s">
-        <v>1393</v>
-      </c>
-      <c r="C1389">
-        <v>7</v>
-      </c>
-      <c r="D1389">
-        <v>450</v>
-      </c>
-      <c r="E1389">
-        <v>125</v>
-      </c>
-      <c r="F1389">
-        <v>-325</v>
-      </c>
-      <c r="G1389">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="1390" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1390" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1390" t="s">
-        <v>1394</v>
-      </c>
-      <c r="C1390">
-        <v>7</v>
-      </c>
-      <c r="D1390">
-        <v>467</v>
-      </c>
-      <c r="E1390">
-        <v>135</v>
-      </c>
-      <c r="F1390">
-        <v>-332</v>
-      </c>
-      <c r="G1390">
-        <v>-99</v>
-      </c>
-    </row>
-    <row r="1391" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1391" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1391" t="s">
-        <v>1395</v>
-      </c>
-      <c r="C1391">
-        <v>7</v>
-      </c>
-      <c r="D1391">
-        <v>463</v>
-      </c>
-      <c r="E1391">
-        <v>133</v>
-      </c>
-      <c r="F1391">
-        <v>-330</v>
-      </c>
-      <c r="G1391">
-        <v>-99</v>
-      </c>
-    </row>
-    <row r="1392" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1392" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1392" t="s">
-        <v>1396</v>
-      </c>
-      <c r="C1392">
-        <v>7</v>
-      </c>
-      <c r="D1392">
-        <v>450</v>
-      </c>
-      <c r="E1392">
-        <v>129</v>
-      </c>
-      <c r="F1392">
-        <v>-321</v>
-      </c>
-      <c r="G1392">
-        <v>-96</v>
-      </c>
-    </row>
-    <row r="1393" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1393" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1393" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C1393">
-        <v>7</v>
-      </c>
-      <c r="D1393">
-        <v>446</v>
-      </c>
-      <c r="E1393">
-        <v>124</v>
-      </c>
-      <c r="F1393">
-        <v>-322</v>
-      </c>
-      <c r="G1393">
-        <v>-99</v>
-      </c>
-    </row>
-    <row r="1394" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1394" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1394" t="s">
-        <v>1398</v>
-      </c>
-      <c r="C1394">
-        <v>7</v>
-      </c>
-      <c r="D1394">
-        <v>393</v>
-      </c>
-      <c r="E1394">
-        <v>129</v>
-      </c>
-      <c r="F1394">
-        <v>-264</v>
-      </c>
-      <c r="G1394">
-        <v>-68</v>
-      </c>
-    </row>
-    <row r="1395" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1395" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1395" t="s">
-        <v>1399</v>
-      </c>
-      <c r="C1395">
-        <v>7</v>
-      </c>
-      <c r="D1395">
-        <v>399</v>
-      </c>
-      <c r="E1395">
-        <v>139</v>
-      </c>
-      <c r="F1395">
-        <v>-260</v>
-      </c>
-      <c r="G1395">
-        <v>-61</v>
-      </c>
-    </row>
-    <row r="1396" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1396" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1396" t="s">
-        <v>1400</v>
-      </c>
-      <c r="C1396">
-        <v>7</v>
-      </c>
-      <c r="D1396">
-        <v>410</v>
-      </c>
-      <c r="E1396">
-        <v>144</v>
-      </c>
-      <c r="F1396">
-        <v>-266</v>
-      </c>
-      <c r="G1396">
-        <v>-61</v>
-      </c>
-    </row>
-    <row r="1397" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1397" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1397" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C1397">
-        <v>7</v>
-      </c>
-      <c r="D1397">
-        <v>426</v>
-      </c>
-      <c r="E1397">
-        <v>145</v>
-      </c>
-      <c r="F1397">
-        <v>-281</v>
-      </c>
-      <c r="G1397">
-        <v>-68</v>
-      </c>
-    </row>
-    <row r="1398" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1398" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1398" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C1398">
-        <v>7</v>
-      </c>
-      <c r="D1398">
-        <v>441</v>
-      </c>
-      <c r="E1398">
-        <v>147</v>
-      </c>
-      <c r="F1398">
-        <v>-294</v>
-      </c>
-      <c r="G1398">
-        <v>-74</v>
-      </c>
-    </row>
-    <row r="1399" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1399" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1399" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C1399">
-        <v>7</v>
-      </c>
-      <c r="D1399">
-        <v>448</v>
-      </c>
-      <c r="E1399">
-        <v>149</v>
-      </c>
-      <c r="F1399">
-        <v>-299</v>
-      </c>
-      <c r="G1399">
-        <v>-75</v>
-      </c>
-    </row>
-    <row r="1400" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1400" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1400" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C1400">
-        <v>7</v>
-      </c>
-      <c r="D1400">
-        <v>453</v>
-      </c>
-      <c r="E1400">
-        <v>150</v>
-      </c>
-      <c r="F1400">
-        <v>-303</v>
-      </c>
-      <c r="G1400">
-        <v>-77</v>
-      </c>
-    </row>
-    <row r="1401" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1401" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1401" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C1401">
-        <v>7</v>
-      </c>
-      <c r="D1401">
-        <v>468</v>
-      </c>
-      <c r="E1401">
-        <v>153</v>
-      </c>
-      <c r="F1401">
-        <v>-315</v>
-      </c>
-      <c r="G1401">
-        <v>-81</v>
-      </c>
-    </row>
-    <row r="1402" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1402" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1402" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C1402">
-        <v>7</v>
-      </c>
-      <c r="D1402">
-        <v>477</v>
-      </c>
-      <c r="E1402">
-        <v>166</v>
-      </c>
-      <c r="F1402">
-        <v>-311</v>
-      </c>
-      <c r="G1402">
-        <v>-73</v>
-      </c>
-    </row>
-    <row r="1403" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1403" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1403" t="s">
-        <v>1407</v>
-      </c>
-      <c r="C1403">
-        <v>7</v>
-      </c>
-      <c r="D1403">
-        <v>483</v>
-      </c>
-      <c r="E1403">
-        <v>176</v>
-      </c>
-      <c r="F1403">
-        <v>-307</v>
-      </c>
-      <c r="G1403">
-        <v>-66</v>
-      </c>
-    </row>
-    <row r="1404" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1404" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1404" t="s">
-        <v>1408</v>
-      </c>
-      <c r="C1404">
-        <v>7</v>
-      </c>
-      <c r="D1404">
-        <v>433</v>
-      </c>
-      <c r="E1404">
-        <v>182</v>
-      </c>
-      <c r="F1404">
-        <v>-251</v>
-      </c>
-      <c r="G1404">
-        <v>-35</v>
-      </c>
-    </row>
-    <row r="1405" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1405" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1405" t="s">
-        <v>1409</v>
-      </c>
-      <c r="C1405">
-        <v>7</v>
-      </c>
-      <c r="D1405">
-        <v>401</v>
-      </c>
-      <c r="E1405">
-        <v>182</v>
-      </c>
-      <c r="F1405">
-        <v>-219</v>
-      </c>
-      <c r="G1405">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="1406" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1406" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1406" t="s">
-        <v>1410</v>
-      </c>
-      <c r="C1406">
-        <v>7</v>
-      </c>
-      <c r="D1406">
-        <v>391</v>
-      </c>
-      <c r="E1406">
-        <v>182</v>
-      </c>
-      <c r="F1406">
-        <v>-209</v>
-      </c>
-      <c r="G1406">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="1407" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1407" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1407" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C1407">
-        <v>7</v>
-      </c>
-      <c r="D1407">
-        <v>387</v>
-      </c>
-      <c r="E1407">
-        <v>167</v>
-      </c>
-      <c r="F1407">
-        <v>-220</v>
-      </c>
-      <c r="G1407">
-        <v>-27</v>
-      </c>
-    </row>
-    <row r="1408" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1408" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1408" t="s">
-        <v>1412</v>
-      </c>
-      <c r="C1408">
-        <v>7</v>
-      </c>
-      <c r="D1408">
-        <v>378</v>
-      </c>
-      <c r="E1408">
-        <v>152</v>
-      </c>
-      <c r="F1408">
-        <v>-226</v>
-      </c>
-      <c r="G1408">
-        <v>-37</v>
-      </c>
-    </row>
-    <row r="1409" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1409" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1409" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C1409">
-        <v>7</v>
-      </c>
-      <c r="D1409">
-        <v>354</v>
-      </c>
-      <c r="E1409">
-        <v>147</v>
-      </c>
-      <c r="F1409">
-        <v>-207</v>
-      </c>
-      <c r="G1409">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="1410" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1410" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1410" t="s">
-        <v>1414</v>
-      </c>
-      <c r="C1410">
-        <v>7</v>
-      </c>
-      <c r="D1410">
-        <v>343</v>
-      </c>
-      <c r="E1410">
-        <v>145</v>
-      </c>
-      <c r="F1410">
-        <v>-198</v>
-      </c>
-      <c r="G1410">
-        <v>-27</v>
-      </c>
-    </row>
-    <row r="1411" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1411" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1411" t="s">
-        <v>1415</v>
-      </c>
-      <c r="C1411">
-        <v>7</v>
-      </c>
-      <c r="D1411">
-        <v>350</v>
-      </c>
-      <c r="E1411">
-        <v>152</v>
-      </c>
-      <c r="F1411">
-        <v>-198</v>
-      </c>
-      <c r="G1411">
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="1412" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1412" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1412" t="s">
-        <v>1416</v>
-      </c>
-      <c r="C1412">
-        <v>7</v>
-      </c>
-      <c r="D1412">
-        <v>346</v>
-      </c>
-      <c r="E1412">
-        <v>149</v>
-      </c>
-      <c r="F1412">
-        <v>-197</v>
-      </c>
-      <c r="G1412">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="1413" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1413" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1413" t="s">
-        <v>1417</v>
-      </c>
-      <c r="C1413">
-        <v>7</v>
-      </c>
-      <c r="D1413">
-        <v>347</v>
-      </c>
-      <c r="E1413">
-        <v>158</v>
-      </c>
-      <c r="F1413">
-        <v>-189</v>
-      </c>
-      <c r="G1413">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="1414" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1414" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1414" t="s">
-        <v>1418</v>
-      </c>
-      <c r="C1414">
-        <v>7</v>
-      </c>
-      <c r="D1414">
-        <v>344</v>
-      </c>
-      <c r="E1414">
-        <v>158</v>
-      </c>
-      <c r="F1414">
-        <v>-186</v>
-      </c>
-      <c r="G1414">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="1415" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1415" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1415" t="s">
-        <v>1419</v>
-      </c>
-      <c r="C1415">
-        <v>7</v>
-      </c>
-      <c r="D1415">
-        <v>332</v>
-      </c>
-      <c r="E1415">
-        <v>157</v>
-      </c>
-      <c r="F1415">
-        <v>-175</v>
-      </c>
-      <c r="G1415">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="1416" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1416" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1416" t="s">
-        <v>1420</v>
-      </c>
-      <c r="C1416">
-        <v>7</v>
-      </c>
-      <c r="D1416">
-        <v>331</v>
-      </c>
-      <c r="E1416">
-        <v>155</v>
-      </c>
-      <c r="F1416">
-        <v>-176</v>
-      </c>
-      <c r="G1416">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="1417" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1417" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1417" t="s">
-        <v>1421</v>
-      </c>
-      <c r="C1417">
-        <v>7</v>
-      </c>
-      <c r="D1417">
-        <v>331</v>
-      </c>
-      <c r="E1417">
-        <v>156</v>
-      </c>
-      <c r="F1417">
-        <v>-175</v>
-      </c>
-      <c r="G1417">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="1418" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1418" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1418" t="s">
-        <v>1422</v>
-      </c>
-      <c r="C1418">
-        <v>7</v>
-      </c>
-      <c r="D1418">
-        <v>327</v>
-      </c>
-      <c r="E1418">
-        <v>151</v>
-      </c>
-      <c r="F1418">
-        <v>-176</v>
-      </c>
-      <c r="G1418">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="1419" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1419" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1419" t="s">
-        <v>1423</v>
-      </c>
-      <c r="C1419">
-        <v>7</v>
-      </c>
-      <c r="D1419">
-        <v>318</v>
-      </c>
-      <c r="E1419">
-        <v>145</v>
-      </c>
-      <c r="F1419">
-        <v>-173</v>
-      </c>
-      <c r="G1419">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="1420" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1420" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1420" t="s">
-        <v>1424</v>
-      </c>
-      <c r="C1420">
-        <v>7</v>
-      </c>
-      <c r="D1420">
-        <v>309</v>
-      </c>
-      <c r="E1420">
-        <v>136</v>
-      </c>
-      <c r="F1420">
-        <v>-173</v>
-      </c>
-      <c r="G1420">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="1421" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1421" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1421" t="s">
-        <v>1425</v>
-      </c>
-      <c r="C1421">
-        <v>7</v>
-      </c>
-      <c r="D1421">
-        <v>305</v>
-      </c>
-      <c r="E1421">
-        <v>134</v>
-      </c>
-      <c r="F1421">
-        <v>-171</v>
-      </c>
-      <c r="G1421">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="1422" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1422" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1422" t="s">
-        <v>1426</v>
-      </c>
-      <c r="C1422">
-        <v>7</v>
-      </c>
-      <c r="D1422">
-        <v>308</v>
-      </c>
-      <c r="E1422">
-        <v>145</v>
-      </c>
-      <c r="F1422">
-        <v>-163</v>
-      </c>
-      <c r="G1422">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="1423" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1423" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1423" t="s">
-        <v>1427</v>
-      </c>
-      <c r="C1423">
-        <v>7</v>
-      </c>
-      <c r="D1423">
-        <v>322</v>
-      </c>
-      <c r="E1423">
-        <v>153</v>
-      </c>
-      <c r="F1423">
-        <v>-169</v>
-      </c>
-      <c r="G1423">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="1424" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1424" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1424" t="s">
-        <v>1428</v>
-      </c>
-      <c r="C1424">
-        <v>7</v>
-      </c>
-      <c r="D1424">
-        <v>337</v>
-      </c>
-      <c r="E1424">
-        <v>159</v>
-      </c>
-      <c r="F1424">
-        <v>-178</v>
-      </c>
-      <c r="G1424">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="1425" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1425" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1425" t="s">
-        <v>1429</v>
-      </c>
-      <c r="C1425">
-        <v>7</v>
-      </c>
-      <c r="D1425">
-        <v>342</v>
-      </c>
-      <c r="E1425">
-        <v>158</v>
-      </c>
-      <c r="F1425">
-        <v>-184</v>
-      </c>
-      <c r="G1425">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="1426" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1426" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1426" t="s">
-        <v>1430</v>
-      </c>
-      <c r="C1426">
-        <v>7</v>
-      </c>
-      <c r="D1426">
-        <v>349</v>
-      </c>
-      <c r="E1426">
-        <v>156</v>
-      </c>
-      <c r="F1426">
-        <v>-193</v>
-      </c>
-      <c r="G1426">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="1427" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1427" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1427" t="s">
-        <v>1431</v>
-      </c>
-      <c r="C1427">
-        <v>7</v>
-      </c>
-      <c r="D1427">
-        <v>350</v>
-      </c>
-      <c r="E1427">
-        <v>152</v>
-      </c>
-      <c r="F1427">
-        <v>-198</v>
-      </c>
-      <c r="G1427">
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="1428" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1428" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1428" t="s">
-        <v>1432</v>
-      </c>
-      <c r="C1428">
-        <v>7</v>
-      </c>
-      <c r="D1428">
-        <v>341</v>
-      </c>
-      <c r="E1428">
-        <v>145</v>
-      </c>
-      <c r="F1428">
-        <v>-196</v>
-      </c>
-      <c r="G1428">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="1429" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1429" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1429" t="s">
-        <v>1433</v>
-      </c>
-      <c r="C1429">
-        <v>7</v>
-      </c>
-      <c r="D1429">
-        <v>333</v>
-      </c>
-      <c r="E1429">
-        <v>140</v>
-      </c>
-      <c r="F1429">
-        <v>-193</v>
-      </c>
-      <c r="G1429">
-        <v>-27</v>
-      </c>
-    </row>
-    <row r="1430" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1430" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1430" t="s">
-        <v>1434</v>
-      </c>
-      <c r="C1430">
-        <v>7</v>
-      </c>
-      <c r="D1430">
-        <v>334</v>
-      </c>
-      <c r="E1430">
-        <v>141</v>
-      </c>
-      <c r="F1430">
-        <v>-193</v>
-      </c>
-      <c r="G1430">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="1431" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1431" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1431" t="s">
-        <v>1435</v>
-      </c>
-      <c r="C1431">
-        <v>7</v>
-      </c>
-      <c r="D1431">
-        <v>334</v>
-      </c>
-      <c r="E1431">
-        <v>142</v>
-      </c>
-      <c r="F1431">
-        <v>-192</v>
-      </c>
-      <c r="G1431">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="1432" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1432" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1432" t="s">
-        <v>1436</v>
-      </c>
-      <c r="C1432">
-        <v>7</v>
-      </c>
-      <c r="D1432">
-        <v>328</v>
-      </c>
-      <c r="E1432">
-        <v>141</v>
-      </c>
-      <c r="F1432">
-        <v>-187</v>
-      </c>
-      <c r="G1432">
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="1433" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1433" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1433" t="s">
-        <v>1437</v>
-      </c>
-      <c r="C1433">
-        <v>7</v>
-      </c>
-      <c r="D1433">
-        <v>322</v>
-      </c>
-      <c r="E1433">
-        <v>141</v>
-      </c>
-      <c r="F1433">
-        <v>-181</v>
-      </c>
-      <c r="G1433">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="1434" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1434" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1434" t="s">
-        <v>1438</v>
-      </c>
-      <c r="C1434">
-        <v>7</v>
-      </c>
-      <c r="D1434">
-        <v>321</v>
-      </c>
-      <c r="E1434">
-        <v>135</v>
-      </c>
-      <c r="F1434">
-        <v>-186</v>
-      </c>
-      <c r="G1434">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="1435" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1435" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1435" t="s">
-        <v>1439</v>
-      </c>
-      <c r="C1435">
-        <v>7</v>
-      </c>
-      <c r="D1435">
-        <v>318</v>
-      </c>
-      <c r="E1435">
-        <v>134</v>
-      </c>
-      <c r="F1435">
-        <v>-184</v>
-      </c>
-      <c r="G1435">
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="1436" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1436" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1436" t="s">
-        <v>1440</v>
-      </c>
-      <c r="C1436">
-        <v>7</v>
-      </c>
-      <c r="D1436">
-        <v>317</v>
-      </c>
-      <c r="E1436">
-        <v>136</v>
-      </c>
-      <c r="F1436">
-        <v>-181</v>
-      </c>
-      <c r="G1436">
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="1437" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1437" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1437" t="s">
-        <v>1441</v>
-      </c>
-      <c r="C1437">
-        <v>7</v>
-      </c>
-      <c r="D1437">
-        <v>312</v>
-      </c>
-      <c r="E1437">
-        <v>138</v>
-      </c>
-      <c r="F1437">
-        <v>-174</v>
-      </c>
-      <c r="G1437">
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="1438" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1438" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1438" t="s">
-        <v>1442</v>
-      </c>
-      <c r="C1438">
-        <v>7</v>
-      </c>
-      <c r="D1438">
-        <v>305</v>
-      </c>
-      <c r="E1438">
-        <v>134</v>
-      </c>
-      <c r="F1438">
-        <v>-171</v>
-      </c>
-      <c r="G1438">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="1439" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1439" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1439" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C1439">
-        <v>7</v>
-      </c>
-      <c r="D1439">
-        <v>304</v>
-      </c>
-      <c r="E1439">
-        <v>132</v>
-      </c>
-      <c r="F1439">
-        <v>-172</v>
-      </c>
-      <c r="G1439">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="1440" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1440" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1440" t="s">
-        <v>1444</v>
-      </c>
-      <c r="C1440">
-        <v>7</v>
-      </c>
-      <c r="D1440">
-        <v>304</v>
-      </c>
-      <c r="E1440">
-        <v>135</v>
-      </c>
-      <c r="F1440">
-        <v>-169</v>
-      </c>
-      <c r="G1440">
-        <v>-17</v>
-      </c>
-    </row>
-    <row r="1441" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1441" s="2">
-        <v>41646</v>
-      </c>
-      <c r="B1441" t="s">
-        <v>1445</v>
-      </c>
-      <c r="C1441">
-        <v>7</v>
-      </c>
-      <c r="D1441">
-        <v>288</v>
-      </c>
-      <c r="E1441">
-        <v>129</v>
-      </c>
-      <c r="F1441">
-        <v>-159</v>
-      </c>
-      <c r="G1441">
-        <v>-15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>